<commit_message>
Perfect the comment to create Help API.
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/Keywordscripts/600.60.20.40_ServerOptionsViewandStoreAlarms.xlsx
+++ b/NformTester/NformTester/Keywordscripts/600.60.20.40_ServerOptionsViewandStoreAlarms.xlsx
@@ -3821,10 +3821,6 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>F</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
     <t>FormManaged_Devices</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -4046,6 +4042,10 @@
   </si>
   <si>
     <t>"1,000"</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>;</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -4633,8 +4633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C127" sqref="C127"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4792,7 +4792,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -4816,32 +4816,32 @@
         <v>5</v>
       </c>
       <c r="D6" s="19" t="s">
+        <v>903</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>845</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="F6" s="17" t="s">
         <v>846</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>847</v>
       </c>
       <c r="G6" s="17"/>
       <c r="H6" s="17" t="s">
+        <v>847</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>885</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>857</v>
+      </c>
+      <c r="K6" s="17" t="s">
         <v>848</v>
       </c>
-      <c r="I6" s="20" t="s">
-        <v>886</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>858</v>
-      </c>
-      <c r="K6" s="17" t="s">
+      <c r="L6" s="17" t="s">
         <v>849</v>
       </c>
-      <c r="L6" s="17" t="s">
+      <c r="M6" s="17" t="s">
         <v>850</v>
-      </c>
-      <c r="M6" s="17" t="s">
-        <v>851</v>
       </c>
       <c r="N6" s="23"/>
     </row>
@@ -4856,7 +4856,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
@@ -4978,10 +4978,10 @@
         <v>7</v>
       </c>
       <c r="H11" s="20" t="s">
+        <v>852</v>
+      </c>
+      <c r="I11" s="17" t="s">
         <v>853</v>
-      </c>
-      <c r="I11" s="17" t="s">
-        <v>854</v>
       </c>
       <c r="J11" s="17" t="b">
         <v>1</v>
@@ -5013,10 +5013,10 @@
         <v>7</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="J12" s="17">
         <v>500</v>
@@ -5048,7 +5048,7 @@
         <v>4</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="I13" s="17"/>
       <c r="J13" s="17"/>
@@ -5195,10 +5195,10 @@
         <v>7</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="I18" s="17" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="J18" s="17">
         <v>10</v>
@@ -5230,7 +5230,7 @@
         <v>4</v>
       </c>
       <c r="H19" s="20" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="I19" s="17"/>
       <c r="J19" s="17"/>
@@ -5375,10 +5375,10 @@
         <v>7</v>
       </c>
       <c r="H24" s="20" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="I24" s="17" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="J24" s="17">
         <v>10</v>
@@ -5408,7 +5408,7 @@
         <v>4</v>
       </c>
       <c r="H25" s="20" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="I25" s="17"/>
       <c r="J25" s="17"/>
@@ -5530,10 +5530,10 @@
         <v>7</v>
       </c>
       <c r="H30" s="20" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="I30" s="17" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="J30" s="17">
         <v>10</v>
@@ -5560,7 +5560,7 @@
         <v>4</v>
       </c>
       <c r="H31" s="20" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="I31" s="17"/>
       <c r="J31" s="17"/>
@@ -5682,10 +5682,10 @@
         <v>7</v>
       </c>
       <c r="H36" s="20" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="I36" s="17" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="J36" s="17">
         <v>10</v>
@@ -5712,7 +5712,7 @@
         <v>4</v>
       </c>
       <c r="H37" s="20" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="I37" s="17"/>
       <c r="J37" s="17"/>
@@ -5834,10 +5834,10 @@
         <v>7</v>
       </c>
       <c r="H42" s="20" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="I42" s="17" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="J42" s="17">
         <v>5000</v>
@@ -5864,7 +5864,7 @@
         <v>4</v>
       </c>
       <c r="H43" s="20" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="I43" s="17"/>
       <c r="J43" s="17"/>
@@ -5902,7 +5902,7 @@
         <v>44</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="E45" s="20"/>
       <c r="F45" s="17"/>
@@ -5968,13 +5968,13 @@
         <v>47</v>
       </c>
       <c r="D48" s="19" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="E48" s="20" t="s">
         <v>19</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G48" s="17" t="s">
         <v>2</v>
@@ -5998,13 +5998,13 @@
         <v>19</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G49" s="17" t="s">
         <v>3</v>
       </c>
       <c r="H49" s="17" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="I49" s="20"/>
       <c r="J49" s="17"/>
@@ -6042,7 +6042,7 @@
         <v>50</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="E51" s="20"/>
       <c r="F51" s="3"/>
@@ -6060,7 +6060,7 @@
         <v>51</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="E52" s="20" t="s">
         <v>802</v>
@@ -6068,13 +6068,13 @@
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="20" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="I52" s="20">
         <v>15</v>
       </c>
       <c r="J52" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
@@ -6086,10 +6086,10 @@
         <v>52</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="E53" s="20" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="F53" s="3">
         <v>10</v>
@@ -6108,7 +6108,7 @@
         <v>53</v>
       </c>
       <c r="D54" s="13" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="E54" s="20"/>
       <c r="F54" s="17"/>
@@ -6126,10 +6126,10 @@
         <v>54</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="E55" s="20" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="F55" s="3">
         <v>5</v>
@@ -6148,7 +6148,7 @@
         <v>55</v>
       </c>
       <c r="D56" s="13" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="E56" s="20"/>
       <c r="F56" s="17"/>
@@ -6250,10 +6250,10 @@
         <v>7</v>
       </c>
       <c r="H60" s="20" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="I60" s="17" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="J60" s="17" t="b">
         <v>0</v>
@@ -6304,13 +6304,13 @@
         <v>7</v>
       </c>
       <c r="H62" s="20" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="I62" s="20" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="J62" s="17" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="K62" s="17"/>
       <c r="L62" s="17"/>
@@ -6334,7 +6334,7 @@
         <v>13</v>
       </c>
       <c r="H63" s="17" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="I63" s="17"/>
       <c r="J63" s="17"/>
@@ -6354,10 +6354,10 @@
         <v>437</v>
       </c>
       <c r="F64" s="17" t="s">
+        <v>876</v>
+      </c>
+      <c r="G64" s="17" t="s">
         <v>877</v>
-      </c>
-      <c r="G64" s="17" t="s">
-        <v>878</v>
       </c>
       <c r="H64" s="20"/>
       <c r="I64" s="17"/>
@@ -6372,7 +6372,7 @@
         <v>64</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="E65" s="20"/>
       <c r="F65" s="17"/>
@@ -6444,7 +6444,7 @@
         <v>19</v>
       </c>
       <c r="F68" s="20" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G68" s="17" t="s">
         <v>2</v>
@@ -6468,13 +6468,13 @@
         <v>19</v>
       </c>
       <c r="F69" s="20" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G69" s="17" t="s">
         <v>3</v>
       </c>
       <c r="H69" s="17" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="I69" s="20"/>
       <c r="J69" s="17"/>
@@ -6512,7 +6512,7 @@
         <v>70</v>
       </c>
       <c r="D71" s="13" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="E71" s="20"/>
       <c r="F71" s="3"/>
@@ -6530,7 +6530,7 @@
         <v>71</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="E72" s="20" t="s">
         <v>802</v>
@@ -6538,13 +6538,13 @@
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
       <c r="H72" s="20" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="I72" s="20">
         <v>10</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
@@ -6556,10 +6556,10 @@
         <v>72</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="E73" s="20" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="F73" s="3">
         <v>10</v>
@@ -6578,7 +6578,7 @@
         <v>73</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="E74" s="20"/>
       <c r="F74" s="17"/>
@@ -6650,7 +6650,7 @@
         <v>19</v>
       </c>
       <c r="F77" s="20" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G77" s="17" t="s">
         <v>2</v>
@@ -6674,7 +6674,7 @@
         <v>19</v>
       </c>
       <c r="F78" s="20" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G78" s="3" t="s">
         <v>58</v>
@@ -6723,7 +6723,7 @@
         <v>830</v>
       </c>
       <c r="E80" s="20" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="F80" s="20" t="s">
         <v>465</v>
@@ -6732,13 +6732,13 @@
         <v>7</v>
       </c>
       <c r="H80" s="20" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="I80" s="20" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="J80" s="17" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="K80" s="17"/>
       <c r="L80" s="17"/>
@@ -6753,19 +6753,19 @@
         <v>830</v>
       </c>
       <c r="E81" s="20" t="s">
+        <v>879</v>
+      </c>
+      <c r="F81" s="17" t="s">
         <v>880</v>
       </c>
-      <c r="F81" s="17" t="s">
-        <v>881</v>
-      </c>
       <c r="G81" s="17" t="s">
         <v>7</v>
       </c>
       <c r="H81" s="20" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="I81" s="20" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="J81" s="17" t="b">
         <v>1</v>
@@ -6783,7 +6783,7 @@
         <v>830</v>
       </c>
       <c r="E82" s="20" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="F82" s="3" t="s">
         <v>100</v>
@@ -6804,7 +6804,7 @@
         <v>82</v>
       </c>
       <c r="D83" s="13" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="E83" s="20"/>
       <c r="F83" s="17"/>
@@ -6906,10 +6906,10 @@
         <v>7</v>
       </c>
       <c r="H87" s="20" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="I87" s="17" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="J87" s="17" t="b">
         <v>1</v>
@@ -6960,13 +6960,13 @@
         <v>7</v>
       </c>
       <c r="H89" s="20" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="I89" s="20" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="J89" s="17" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="K89" s="17"/>
       <c r="L89" s="17"/>
@@ -6990,7 +6990,7 @@
         <v>13</v>
       </c>
       <c r="H90" s="17" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="I90" s="17"/>
       <c r="J90" s="17"/>
@@ -7010,10 +7010,10 @@
         <v>437</v>
       </c>
       <c r="F91" s="17" t="s">
+        <v>876</v>
+      </c>
+      <c r="G91" s="17" t="s">
         <v>877</v>
-      </c>
-      <c r="G91" s="17" t="s">
-        <v>878</v>
       </c>
       <c r="H91" s="20"/>
       <c r="I91" s="17"/>
@@ -7028,7 +7028,7 @@
         <v>91</v>
       </c>
       <c r="D92" s="13" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="E92" s="20"/>
       <c r="F92" s="17"/>
@@ -7100,7 +7100,7 @@
         <v>19</v>
       </c>
       <c r="F95" s="20" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G95" s="17" t="s">
         <v>2</v>
@@ -7124,13 +7124,13 @@
         <v>19</v>
       </c>
       <c r="F96" s="20" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G96" s="17" t="s">
         <v>3</v>
       </c>
       <c r="H96" s="17" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="I96" s="20"/>
       <c r="J96" s="17"/>
@@ -7168,7 +7168,7 @@
         <v>97</v>
       </c>
       <c r="D98" s="13" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="E98" s="20"/>
       <c r="F98" s="3"/>
@@ -7186,7 +7186,7 @@
         <v>98</v>
       </c>
       <c r="D99" s="11" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="E99" s="20" t="s">
         <v>802</v>
@@ -7194,13 +7194,13 @@
       <c r="F99" s="3"/>
       <c r="G99" s="3"/>
       <c r="H99" s="20" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="I99" s="20">
         <v>10</v>
       </c>
       <c r="J99" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
@@ -7212,10 +7212,10 @@
         <v>99</v>
       </c>
       <c r="D100" s="11" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="E100" s="20" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="F100" s="3">
         <v>10</v>
@@ -7234,7 +7234,7 @@
         <v>100</v>
       </c>
       <c r="D101" s="13" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="E101" s="20"/>
       <c r="F101" s="17"/>
@@ -7306,7 +7306,7 @@
         <v>19</v>
       </c>
       <c r="F104" s="20" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G104" s="17" t="s">
         <v>2</v>
@@ -7330,7 +7330,7 @@
         <v>19</v>
       </c>
       <c r="F105" s="20" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G105" s="3" t="s">
         <v>58</v>
@@ -7379,7 +7379,7 @@
         <v>830</v>
       </c>
       <c r="E107" s="20" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="F107" s="20" t="s">
         <v>465</v>
@@ -7388,13 +7388,13 @@
         <v>7</v>
       </c>
       <c r="H107" s="20" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="I107" s="20" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="J107" s="17" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="K107" s="17"/>
       <c r="L107" s="17"/>
@@ -7409,19 +7409,19 @@
         <v>830</v>
       </c>
       <c r="E108" s="20" t="s">
+        <v>879</v>
+      </c>
+      <c r="F108" s="17" t="s">
         <v>880</v>
       </c>
-      <c r="F108" s="17" t="s">
-        <v>881</v>
-      </c>
       <c r="G108" s="17" t="s">
         <v>7</v>
       </c>
       <c r="H108" s="20" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="I108" s="20" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="J108" s="17" t="b">
         <v>0</v>
@@ -7439,7 +7439,7 @@
         <v>830</v>
       </c>
       <c r="E109" s="20" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="F109" s="3" t="s">
         <v>100</v>
@@ -7460,7 +7460,7 @@
         <v>109</v>
       </c>
       <c r="D110" s="13" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="E110" s="20"/>
       <c r="F110" s="3"/>
@@ -7562,13 +7562,13 @@
         <v>7</v>
       </c>
       <c r="H114" s="20" t="s">
+        <v>891</v>
+      </c>
+      <c r="I114" s="17" t="s">
+        <v>853</v>
+      </c>
+      <c r="J114" s="17" t="s">
         <v>892</v>
-      </c>
-      <c r="I114" s="17" t="s">
-        <v>854</v>
-      </c>
-      <c r="J114" s="17" t="s">
-        <v>893</v>
       </c>
       <c r="K114" s="17"/>
       <c r="L114" s="17"/>
@@ -7592,13 +7592,13 @@
         <v>7</v>
       </c>
       <c r="H115" s="20" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="I115" s="17" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="J115" s="17" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="K115" s="17"/>
       <c r="L115" s="17"/>
@@ -7622,13 +7622,13 @@
         <v>7</v>
       </c>
       <c r="H116" s="20" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="I116" s="17" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="J116" s="17" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="K116" s="17"/>
       <c r="L116" s="17"/>
@@ -7652,10 +7652,10 @@
         <v>7</v>
       </c>
       <c r="H117" s="20" t="s">
+        <v>852</v>
+      </c>
+      <c r="I117" s="17" t="s">
         <v>853</v>
-      </c>
-      <c r="I117" s="17" t="s">
-        <v>854</v>
       </c>
       <c r="J117" s="17" t="b">
         <v>0</v>
@@ -7682,7 +7682,7 @@
         <v>4</v>
       </c>
       <c r="H118" s="20" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="I118" s="17"/>
       <c r="J118" s="17"/>
@@ -7708,7 +7708,7 @@
         <v>4</v>
       </c>
       <c r="H119" s="20" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="I119" s="17"/>
       <c r="J119" s="17"/>
@@ -7734,7 +7734,7 @@
         <v>4</v>
       </c>
       <c r="H120" s="20" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="I120" s="17"/>
       <c r="J120" s="17"/>
@@ -7856,13 +7856,13 @@
         <v>7</v>
       </c>
       <c r="H125" s="20" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="I125" s="17" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="J125" s="17" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="K125" s="17"/>
       <c r="L125" s="17"/>
@@ -7886,13 +7886,13 @@
         <v>7</v>
       </c>
       <c r="H126" s="20" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="I126" s="17" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="J126" s="17" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="K126" s="17"/>
       <c r="L126" s="17"/>
@@ -7916,13 +7916,13 @@
         <v>7</v>
       </c>
       <c r="H127" s="20" t="s">
+        <v>891</v>
+      </c>
+      <c r="I127" s="17" t="s">
+        <v>853</v>
+      </c>
+      <c r="J127" s="17" t="s">
         <v>892</v>
-      </c>
-      <c r="I127" s="17" t="s">
-        <v>854</v>
-      </c>
-      <c r="J127" s="17" t="s">
-        <v>893</v>
       </c>
       <c r="K127" s="17"/>
       <c r="L127" s="17"/>
@@ -7946,10 +7946,10 @@
         <v>7</v>
       </c>
       <c r="H128" s="20" t="s">
+        <v>852</v>
+      </c>
+      <c r="I128" s="17" t="s">
         <v>853</v>
-      </c>
-      <c r="I128" s="17" t="s">
-        <v>854</v>
       </c>
       <c r="J128" s="17" t="b">
         <v>0</v>
@@ -7976,7 +7976,7 @@
         <v>4</v>
       </c>
       <c r="H129" s="20" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="I129" s="17"/>
       <c r="J129" s="17"/>
@@ -8002,7 +8002,7 @@
         <v>4</v>
       </c>
       <c r="H130" s="20" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="I130" s="17"/>
       <c r="J130" s="17"/>
@@ -8028,7 +8028,7 @@
         <v>4</v>
       </c>
       <c r="H131" s="20" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="I131" s="17"/>
       <c r="J131" s="17"/>
@@ -8150,13 +8150,13 @@
         <v>7</v>
       </c>
       <c r="H136" s="20" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="I136" s="17" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="J136" s="17" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="K136" s="17"/>
       <c r="L136" s="17"/>
@@ -8180,13 +8180,13 @@
         <v>7</v>
       </c>
       <c r="H137" s="20" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="I137" s="17" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="J137" s="17" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="K137" s="17"/>
       <c r="L137" s="17"/>
@@ -8210,13 +8210,13 @@
         <v>7</v>
       </c>
       <c r="H138" s="20" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="I138" s="17" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="J138" s="17" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="K138" s="17"/>
       <c r="L138" s="17"/>
@@ -8240,10 +8240,10 @@
         <v>7</v>
       </c>
       <c r="H139" s="20" t="s">
+        <v>852</v>
+      </c>
+      <c r="I139" s="17" t="s">
         <v>853</v>
-      </c>
-      <c r="I139" s="17" t="s">
-        <v>854</v>
       </c>
       <c r="J139" s="17" t="b">
         <v>0</v>
@@ -8270,7 +8270,7 @@
         <v>4</v>
       </c>
       <c r="H140" s="20" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="I140" s="17"/>
       <c r="J140" s="17"/>
@@ -8296,7 +8296,7 @@
         <v>4</v>
       </c>
       <c r="H141" s="20" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="I141" s="17"/>
       <c r="J141" s="17"/>
@@ -8322,7 +8322,7 @@
         <v>4</v>
       </c>
       <c r="H142" s="20" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="I142" s="17"/>
       <c r="J142" s="17"/>
@@ -8360,7 +8360,7 @@
         <v>143</v>
       </c>
       <c r="D144" s="13" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="E144" s="20"/>
       <c r="F144" s="17"/>
@@ -8462,7 +8462,7 @@
         <v>4</v>
       </c>
       <c r="H148" s="20" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="I148" s="17"/>
       <c r="J148" s="17"/>
@@ -8488,7 +8488,7 @@
         <v>13</v>
       </c>
       <c r="H149" s="17" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="I149" s="20"/>
       <c r="J149" s="17"/>
@@ -8532,10 +8532,10 @@
         <v>437</v>
       </c>
       <c r="F151" s="17" t="s">
+        <v>876</v>
+      </c>
+      <c r="G151" s="17" t="s">
         <v>877</v>
-      </c>
-      <c r="G151" s="17" t="s">
-        <v>878</v>
       </c>
       <c r="H151" s="20"/>
       <c r="I151" s="17"/>
@@ -8598,10 +8598,10 @@
         <v>153</v>
       </c>
       <c r="D154" s="11" t="s">
+        <v>883</v>
+      </c>
+      <c r="E154" s="20" t="s">
         <v>884</v>
-      </c>
-      <c r="E154" s="20" t="s">
-        <v>885</v>
       </c>
       <c r="F154" s="3" t="s">
         <v>621</v>
@@ -8610,7 +8610,7 @@
         <v>3</v>
       </c>
       <c r="H154" s="3" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="I154" s="3"/>
       <c r="J154" s="3"/>
@@ -8624,10 +8624,10 @@
         <v>154</v>
       </c>
       <c r="D155" s="11" t="s">
+        <v>883</v>
+      </c>
+      <c r="E155" s="20" t="s">
         <v>884</v>
-      </c>
-      <c r="E155" s="20" t="s">
-        <v>885</v>
       </c>
       <c r="F155" s="3" t="s">
         <v>213</v>
@@ -8648,7 +8648,7 @@
         <v>155</v>
       </c>
       <c r="D156" s="11" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="E156" s="3" t="s">
         <v>628</v>
@@ -8672,10 +8672,10 @@
         <v>156</v>
       </c>
       <c r="D157" s="11" t="s">
+        <v>883</v>
+      </c>
+      <c r="E157" s="20" t="s">
         <v>884</v>
-      </c>
-      <c r="E157" s="20" t="s">
-        <v>885</v>
       </c>
       <c r="F157" s="3" t="s">
         <v>100</v>

</xml_diff>